<commit_message>
Added P1 test Scenerio
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationProject\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDF3C68-3838-4265-925F-63351B467494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2D661E-5A47-488E-BF60-8742C40C3BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="26" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,24 @@
     <sheet name="addChamp_via_workOrder" sheetId="11" r:id="rId10"/>
     <sheet name="addChamp_via_ViewTask" sheetId="12" r:id="rId11"/>
     <sheet name="addChamp_via_dashBoard2" sheetId="14" r:id="rId12"/>
-    <sheet name="addChamp_via_dashBoard_Error" sheetId="15" r:id="rId13"/>
-    <sheet name="addChamp_via_workOrder_Error" sheetId="16" r:id="rId14"/>
-    <sheet name="addChamp_via_ViewTask_Error" sheetId="17" r:id="rId15"/>
-    <sheet name="addChamp_via_dashBoard2_Error" sheetId="18" r:id="rId16"/>
-    <sheet name="Withdraw_valid_Upi" sheetId="21" r:id="rId17"/>
-    <sheet name="Withdraw_valid_Bank" sheetId="22" r:id="rId18"/>
-    <sheet name="Withdraw_Invalid_Upi" sheetId="23" r:id="rId19"/>
-    <sheet name="Withdraw_Invalid_BankNumber" sheetId="24" r:id="rId20"/>
-    <sheet name="Withdraw_Invalid_BankNumber2" sheetId="25" r:id="rId21"/>
-    <sheet name="Withdraw_Invalid_IFSCcode" sheetId="26" r:id="rId22"/>
-    <sheet name="Withdraw_Short_IFSCcode" sheetId="27" r:id="rId23"/>
-    <sheet name="Withdraw_Invalid_Name" sheetId="30" r:id="rId24"/>
-    <sheet name="Withdraw_Short_Name" sheetId="31" r:id="rId25"/>
-    <sheet name="RequestCredit" sheetId="33" r:id="rId26"/>
-    <sheet name="TaskCredit" sheetId="34" r:id="rId27"/>
+    <sheet name="Sheet1" sheetId="36" r:id="rId13"/>
+    <sheet name="addChamp_via_dashBoard_Error" sheetId="15" r:id="rId14"/>
+    <sheet name="addChamp_via_workOrder_Error" sheetId="16" r:id="rId15"/>
+    <sheet name="addChamp_via_ViewTask_Error" sheetId="17" r:id="rId16"/>
+    <sheet name="addChamp_via_dashBoard2_Error" sheetId="18" r:id="rId17"/>
+    <sheet name="Withdraw_valid_Upi" sheetId="21" r:id="rId18"/>
+    <sheet name="Withdraw_valid_Bank" sheetId="22" r:id="rId19"/>
+    <sheet name="Withdraw_Invalid_Upi" sheetId="23" r:id="rId20"/>
+    <sheet name="Withdraw_Invalid_BankNumber" sheetId="24" r:id="rId21"/>
+    <sheet name="Withdraw_Invalid_BankNumber2" sheetId="25" r:id="rId22"/>
+    <sheet name="CreateworkorderPage" sheetId="35" r:id="rId23"/>
+    <sheet name="Withdraw_Invalid_IFSCcode" sheetId="26" r:id="rId24"/>
+    <sheet name="Withdraw_Short_IFSCcode" sheetId="27" r:id="rId25"/>
+    <sheet name="Withdraw_Invalid_Name" sheetId="30" r:id="rId26"/>
+    <sheet name="Withdraw_Short_Name" sheetId="31" r:id="rId27"/>
+    <sheet name="RequestCredit" sheetId="33" r:id="rId28"/>
+    <sheet name="TaskCredit" sheetId="34" r:id="rId29"/>
+    <sheet name="addChamp_WorkOrder_Vendor" sheetId="37" r:id="rId30"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="73">
   <si>
     <t>phoneOrEmail</t>
   </si>
@@ -233,22 +236,43 @@
     <t>Invalid VPA. Please enter a valid Virtual Payment Address</t>
   </si>
   <si>
-    <t>Please enter valid account number</t>
-  </si>
-  <si>
     <t>Invalid IFSC Code in Bank Account</t>
   </si>
   <si>
     <t>The ifsc must be 11 characters.</t>
   </si>
   <si>
-    <t>Please enter valid account holder name</t>
-  </si>
-  <si>
     <t>The name must be between 3 and 120 characters.</t>
   </si>
   <si>
-    <t>Amount will receive to your bank account soon. . .</t>
+    <t>The account number format is invalid.</t>
+  </si>
+  <si>
+    <t>The name format is invalid.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>expectedSuccessmessage</t>
+  </si>
+  <si>
+    <t>Work order added successfully!</t>
+  </si>
+  <si>
+    <t>kitty</t>
+  </si>
+  <si>
+    <t>08/30/2024</t>
+  </si>
+  <si>
+    <t>virgil.dirk@dockstones.com</t>
+  </si>
+  <si>
+    <t>kasubf374</t>
   </si>
 </sst>
 </file>
@@ -639,10 +663,63 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB04788-F2AA-48AC-9845-332224957FD6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>9200549210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CEAEE-C2F7-4169-8392-080908B37DBD}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,12 +742,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CEAEE-C2F7-4169-8392-080908B37DBD}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7593BD91-A25E-4B84-BB2E-B3EA0B393644}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="BM1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,35 +770,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7593BD91-A25E-4B84-BB2E-B3EA0B393644}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9A4550-9668-4E46-BADA-4A66B7C9AE88}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AB48DE-8D73-4307-BB97-8607CEEC1768}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -749,7 +810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F275F6-97A7-4E8E-9D70-835F9D22710E}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -777,7 +838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD96149-6A7E-4735-9024-63AF7B287546}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -805,7 +866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DED200-7E23-45CA-8D5A-0B2480557A3F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -833,12 +894,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619D10E0-4481-4EF3-8BAD-5AD6EADFA26A}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,12 +987,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38D1885-FF36-4CE0-9730-9534EAF02835}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="M12" activeCellId="1" sqref="J18 M12"/>
+    <sheetView topLeftCell="F1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,7 +1090,7 @@
         <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1103,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB981E43-EC92-4082-87A8-F886F963D720}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2">
+        <v>1234567893</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F1433BDC-8099-4DA1-82C9-B6615CB333D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0207F3-3648-4B2F-87B0-F1F1EFAE37D6}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1108,77 +1234,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB981E43-EC92-4082-87A8-F886F963D720}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>123456</v>
-      </c>
-      <c r="C2">
-        <v>1234567893</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F1433BDC-8099-4DA1-82C9-B6615CB333D7}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD465F8-8ADD-4DD5-8207-7DD7D91A0BEC}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,7 +1309,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1262,12 +1323,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F49695-C608-495A-9A3F-104B112DA8D3}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1343,7 +1404,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A2615BA-CA24-4868-A76E-5A8928E92239}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9957984E-7AB4-43A3-AB84-00D64A6741AE}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1418,7 +1519,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BD5CCB-EBB4-4F8B-8CC6-C722CE447543}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1505,7 +1606,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1517,12 +1618,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E09231-894F-4013-958B-2394E3F65C3E}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1592,7 +1693,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC381A8-2269-464B-9A08-7730A794A532}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1679,7 +1780,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1692,7 +1793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E002A3-5062-4DD2-99EA-9D8EE82F45C2}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1765,7 +1866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF2C054-F8FC-44A2-9B7D-23EF641C826F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1843,7 +1944,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B1" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1879,6 +1980,61 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8381F63D-B8F2-4ADD-8781-C5928866CB0E}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B00CAF42-82E2-42EC-BDD9-211683D2ECF6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C67350F-77ED-4FAF-B015-906CD252BB8E}">
   <dimension ref="A1:C3"/>
@@ -2065,26 +2221,51 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0AA793-B14F-4E74-AA45-5E570B464B83}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>9200549210</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commited changes by yash
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\Test\Apptad-AutomationProject\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD98AC15-4BAD-40E8-8554-6C223F83F2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5A9CCC-7A46-4C27-9557-D0A727778F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5424" yWindow="3540" windowWidth="17280" windowHeight="9960" firstSheet="147" activeTab="148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4404" yWindow="1632" windowWidth="17280" windowHeight="9960" firstSheet="164" activeTab="165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectClientInvalidEnterprise" sheetId="175" r:id="rId1"/>
@@ -169,6 +169,16 @@
     <sheet name="CreateWorkorderNameError" sheetId="190" r:id="rId154"/>
     <sheet name="CreateWorkorderPhoneError" sheetId="191" r:id="rId155"/>
     <sheet name="CreateWorkorderEmailError" sheetId="192" r:id="rId156"/>
+    <sheet name="WorkOrderApprovalEnterprise" sheetId="195" r:id="rId157"/>
+    <sheet name="InvalidFieldNameWorkorder" sheetId="196" r:id="rId158"/>
+    <sheet name="InvalidFrequencyWorkorder" sheetId="197" r:id="rId159"/>
+    <sheet name="InvalidRadiusWorkorder" sheetId="198" r:id="rId160"/>
+    <sheet name="InvalidQuoteWorkorder" sheetId="199" r:id="rId161"/>
+    <sheet name="InvalidTermsWorkorder" sheetId="200" r:id="rId162"/>
+    <sheet name="InvalidLocationWorkorder" sheetId="201" r:id="rId163"/>
+    <sheet name="InvalidDateWorkorder" sheetId="202" r:id="rId164"/>
+    <sheet name="InvalidStarttimeWorkorder" sheetId="203" r:id="rId165"/>
+    <sheet name="InvalidEndtimeWorkorder" sheetId="204" r:id="rId166"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -180,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="268">
   <si>
     <t>phoneOrEmail</t>
   </si>
@@ -977,6 +987,15 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>Please select valid quote valid till</t>
+  </si>
+  <si>
+    <t>Please enter valid terms</t>
+  </si>
+  <si>
+    <t>ExpectedtermsResult</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1006,7 @@
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0;[Red]&quot;₹&quot;\ \-#,##0"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1121,6 +1140,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1143,7 +1167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1180,12 +1204,63 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3344,7 +3419,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:F2">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{6B0936EA-1982-4A1F-BB2B-2EFAD7EAA0DF}"/>
@@ -3612,7 +3687,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD1:AE2">
-    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{2E23724F-9C7E-492A-9416-5F0DDA676034}"/>
@@ -4444,7 +4519,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AC1:AD2">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{0BFAE797-9CB7-4402-8F87-D60F6640FF10}"/>
@@ -5046,7 +5121,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1 D2:H2 K1:L2">
-    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{844409B9-4518-416E-88B9-E71A345CFB12}"/>
@@ -5433,7 +5508,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:F2">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{D8729A09-0592-4A14-9550-D4078BDE0145}"/>
@@ -5706,7 +5781,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE1:AG2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{79EEEF3E-4ED6-432F-B6CA-AC81BEC9534C}"/>
@@ -5722,7 +5797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D6E707-CBE9-4EC6-94BE-F1EEE72A82AF}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -5953,7 +6028,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE1:AG2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{BD801DDD-B84A-4786-A6D0-0EB1217C2202}"/>
@@ -6073,7 +6148,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1 D2:H2 K1:L2">
-    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{09430D94-2145-44CA-9915-005A517E8C23}"/>
@@ -6579,6 +6654,452 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet157.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0B2F4-047B-4272-BBC7-EB74B3867E5F}">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection sqref="A1:AA2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="17.399999999999999">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" t="s">
+        <v>170</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.6">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45537</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45545</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2">
+        <v>50000</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2">
+        <v>123456</v>
+      </c>
+      <c r="V2" s="16">
+        <v>45534</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="V1:X2">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8EFD11BE-7842-4001-BF06-9E2A03A215BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet158.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D972AD-E594-49FA-8899-3B7257EB8B2F}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2">
+        <v>112233</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{A9FAAD29-6507-42A5-8A59-FB1D9F4D0C1D}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{D10033B4-6E81-48A2-9585-95B4DA24711B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet159.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D9E835-1CF7-4778-AEF6-31C21134834F}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2">
+        <v>112233</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E2F51A3C-1D70-4B20-8382-8DAB0621B6AE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE43C135-7B06-42FD-95AB-6750E7B25159}">
   <dimension ref="A1:M2"/>
@@ -6687,11 +7208,1179 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:L2 D1:J1 D2:H2">
-    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{BE94A0D7-0410-452E-9BE2-20E4DF1AFF22}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{C31A25F6-8FE9-4140-AA5F-7A642F089A43}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet160.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16363CA8-BBF5-417B-B68D-D6CC27B45294}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2">
+        <v>112233</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{FDBE5125-FCE3-47FC-BE8C-4BB34E0A06EC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet161.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98210AC1-DFFE-49EB-A969-54F58EDEF08C}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2">
+        <v>112233</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2">
+        <v>50000</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2" t="s">
+        <v>99</v>
+      </c>
+      <c r="V2" t="s">
+        <v>100</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{F3249203-384F-429B-8A94-1BB1B82C4F14}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{ACC94EC6-13BA-4EFB-B230-A92208030638}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{2CECCC39-9F8C-467C-915D-D759F9C9BA5B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet162.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE567E-2364-4F64-B743-9361C4C31C66}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2">
+        <v>112233</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2">
+        <v>50000</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2" t="s">
+        <v>99</v>
+      </c>
+      <c r="V2" t="s">
+        <v>100</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{1133929E-1BCD-4A53-8E67-E566F5BA844C}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{A7EAB2A6-4EAD-4C13-A171-5BBF6549BC7A}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{3047D12D-7AC5-4F87-8BDA-59EE4B814E04}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet163.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F552DD-4358-4113-8E23-30B554DB9E0F}">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="22" max="22" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" t="s">
+        <v>170</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45537</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45545</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2">
+        <v>50000</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2">
+        <v>123456</v>
+      </c>
+      <c r="V2" t="s">
+        <v>180</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="14"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="V1:X2">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{E40B2F07-6B5B-4069-B6D8-6BF264DB2927}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet164.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665E3AA7-CFE3-4CD1-9607-6424F9CB5837}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="23" max="23" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" t="s">
+        <v>170</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45537</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45545</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2">
+        <v>50000</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2">
+        <v>123456</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="V1:X2">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{65A2EF95-BD55-41A9-9797-CF10D01B74B1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet165.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4612362F-1EE6-45A1-BCEE-CE2608F6720E}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="23" max="23" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" t="s">
+        <v>170</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45537</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45545</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2">
+        <v>50000</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2">
+        <v>123456</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="V1:X2">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{AAE3F4FE-CA33-4EA9-9CB2-B49F515725F8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet166.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360695DF-45A8-4981-840F-BD8B6D207950}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="23" max="23" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" t="s">
+        <v>170</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45537</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45545</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2">
+        <v>50000</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2">
+        <v>123456</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="V1:X2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{52770C70-9CEB-4C36-8D40-DB314A2BBBBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6805,7 +8494,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1 D2:H2 K1:L2">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{14FC3AB9-B453-46CA-863D-33761C323DDC}"/>
@@ -6876,10 +8565,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1">
-    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F2">
-    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{0A9FF332-F266-4F06-BD9A-1772A62329B6}"/>
@@ -6948,13 +8637,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1">
-    <cfRule type="duplicateValues" dxfId="24" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E2">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{57223C36-ABF7-4C5E-972E-0360280AE7A2}"/>
@@ -7161,8 +8850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA97BF87-4E2F-43C5-8890-D5F49A3A337E}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection sqref="A1:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8026,8 +9715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8440E1FB-2C78-4BD0-BE8F-157B06AF33D6}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AA2"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection sqref="A1:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8228,7 +9917,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="V1:X2">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{608C7CC8-F075-4A70-BD0C-9C5F01AE4F00}"/>
@@ -8672,7 +10361,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:F2">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{C29BB4E8-D791-4E75-A159-A6681271ABE8}"/>
@@ -8686,7 +10375,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="D1" sqref="D1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8751,12 +10440,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="F2" sqref="D1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
@@ -8812,7 +10502,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="D1" sqref="D1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8954,12 +10644,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="C11:D12"/>
+      <selection activeCell="D1" sqref="D1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -10403,7 +12094,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B1" sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10619,8 +12310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE2FE2E-7F9A-4BD7-AF17-BD45E0B98CA5}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10733,8 +12424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06398D3B-89DE-48F0-AA63-A392FFB90D4F}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11463,10 +13154,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{42855C14-FC85-4C1C-AB4D-7250C8919402}"/>
@@ -11542,10 +13233,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7AD5D74A-9765-48B8-AC31-50E848625BC3}"/>
@@ -11621,10 +13312,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{05C1878F-C482-4723-8A0A-0F5B4B980DA8}"/>
@@ -11700,10 +13391,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B3BB0B30-9B36-4021-9B97-7B125847F859}"/>
@@ -11779,10 +13470,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{46346B06-5FDD-43E4-AA51-EA93781CBE3F}"/>
@@ -11858,10 +13549,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{5C5714FD-5F67-4416-BDC2-45A85C6BAD58}"/>
@@ -11937,10 +13628,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{57B46F63-9A1E-4F83-AD1C-A736E9F1DD80}"/>
@@ -12116,10 +13807,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E2">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{AF23535F-A70C-407A-BB87-F15913EFEB88}"/>

</xml_diff>